<commit_message>
BABA, BIDU updates and more
</commit_message>
<xml_diff>
--- a/BIDU.xlsx
+++ b/BIDU.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Martin\code\models\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shkre\code\models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21042709-26C2-4B33-9308-D23445B707DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78F70B0C-5292-4DB0-A2B2-D5026499712A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8685" yWindow="30" windowWidth="20145" windowHeight="15465" activeTab="1" xr2:uid="{E6509C3E-AEFE-495C-9954-6EF385292148}"/>
+    <workbookView xWindow="-20325" yWindow="0" windowWidth="20100" windowHeight="20985" xr2:uid="{E6509C3E-AEFE-495C-9954-6EF385292148}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="74">
   <si>
     <t>Price</t>
   </si>
@@ -201,12 +201,69 @@
   </si>
   <si>
     <t>iQIYI</t>
+  </si>
+  <si>
+    <t>Q123</t>
+  </si>
+  <si>
+    <t>Q223</t>
+  </si>
+  <si>
+    <t>Q323</t>
+  </si>
+  <si>
+    <t>Q423</t>
+  </si>
+  <si>
+    <t>Q124</t>
+  </si>
+  <si>
+    <t>Q224</t>
+  </si>
+  <si>
+    <t>Q324</t>
+  </si>
+  <si>
+    <t>Q424</t>
+  </si>
+  <si>
+    <t>Q125</t>
+  </si>
+  <si>
+    <t>Q225</t>
+  </si>
+  <si>
+    <t>Q325</t>
+  </si>
+  <si>
+    <t>Q425</t>
+  </si>
+  <si>
+    <t>CEO: Robin Li</t>
+  </si>
+  <si>
+    <t>CFO: Rong Luo</t>
+  </si>
+  <si>
+    <t>Revenue y/y</t>
+  </si>
+  <si>
+    <t>CFFO</t>
+  </si>
+  <si>
+    <t>CapEx</t>
+  </si>
+  <si>
+    <t>FCF</t>
+  </si>
+  <si>
+    <t>IQIYI</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -250,7 +307,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -267,13 +324,20 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="Invisible" pivot="0" table="0" count="0" xr9:uid="{B050C7BF-44BA-4B8E-80E2-6ECF931862A6}"/>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -289,16 +353,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>28575</xdr:colOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>1361</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>28575</xdr:colOff>
-      <xdr:row>46</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>1361</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>87086</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -313,8 +377,58 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6657975" y="57150"/>
-          <a:ext cx="0" cy="7143750"/>
+          <a:off x="12438290" y="0"/>
+          <a:ext cx="0" cy="9231086"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>41</xdr:col>
+      <xdr:colOff>19707</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>26276</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>41</xdr:col>
+      <xdr:colOff>19707</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>29308</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="5" name="Straight Connector 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{94D8B0A8-B969-8598-B935-D3928A278DEB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="25209669" y="26276"/>
+          <a:ext cx="0" cy="8868609"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -341,9 +455,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -381,7 +495,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -487,7 +601,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -629,7 +743,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -637,10 +751,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0ED6D289-974A-40CE-AEFB-C496CBF2CC73}">
-  <dimension ref="K2:M9"/>
+  <dimension ref="B2:M12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -648,72 +762,84 @@
     <col min="11" max="11" width="11.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="11:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
+        <v>73</v>
+      </c>
       <c r="K2" t="s">
         <v>0</v>
       </c>
       <c r="L2">
-        <v>138.16999999999999</v>
-      </c>
-    </row>
-    <row r="3" spans="11:13" x14ac:dyDescent="0.2">
+        <v>92.75</v>
+      </c>
+    </row>
+    <row r="3" spans="2:13" x14ac:dyDescent="0.2">
       <c r="K3" t="s">
         <v>1</v>
       </c>
       <c r="L3" s="1">
-        <f>2767/8</f>
-        <v>345.875</v>
+        <v>2834</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="11:13" x14ac:dyDescent="0.2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="2:13" x14ac:dyDescent="0.2">
       <c r="K4" t="s">
         <v>2</v>
       </c>
       <c r="L4" s="1">
         <f>+L2*L3</f>
-        <v>47789.548749999994</v>
-      </c>
-    </row>
-    <row r="5" spans="11:13" x14ac:dyDescent="0.2">
+        <v>262853.5</v>
+      </c>
+    </row>
+    <row r="5" spans="2:13" x14ac:dyDescent="0.2">
       <c r="K5" t="s">
         <v>52</v>
       </c>
       <c r="L5" s="1">
-        <v>255226</v>
+        <v>280691</v>
       </c>
       <c r="M5" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="11:13" x14ac:dyDescent="0.2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6" spans="2:13" x14ac:dyDescent="0.2">
       <c r="K6" t="s">
         <v>53</v>
       </c>
       <c r="L6" s="1">
-        <v>83627</v>
+        <v>74548</v>
       </c>
       <c r="M6" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="11:13" x14ac:dyDescent="0.2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" spans="2:13" x14ac:dyDescent="0.2">
       <c r="K7" t="s">
         <v>5</v>
       </c>
       <c r="L7" s="1">
         <f>+L4-L5+L6</f>
-        <v>-123809.45125000001</v>
-      </c>
-    </row>
-    <row r="9" spans="11:13" x14ac:dyDescent="0.2">
+        <v>56710.5</v>
+      </c>
+    </row>
+    <row r="9" spans="2:13" x14ac:dyDescent="0.2">
       <c r="K9" t="s">
         <v>6</v>
       </c>
       <c r="L9">
         <v>2000</v>
+      </c>
+    </row>
+    <row r="11" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="K11" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="12" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="K12" t="s">
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -723,28 +849,28 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A74257A8-EE5B-46CF-8076-BD55C12B5BDA}">
-  <dimension ref="A1:N46"/>
+  <dimension ref="A1:BF50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane xSplit="2" ySplit="2" topLeftCell="AH3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="AS48" sqref="AS48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17" customWidth="1"/>
     <col min="3" max="14" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:58" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:58" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>9</v>
       </c>
@@ -784,22 +910,190 @@
       <c r="N2" s="2" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B3" t="s">
+      <c r="O2" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="R2" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="S2" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="T2" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="U2" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="V2" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="W2" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="X2" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="Y2" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="Z2" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="AB2">
+        <v>2010</v>
+      </c>
+      <c r="AC2">
+        <f>+AB2+1</f>
+        <v>2011</v>
+      </c>
+      <c r="AD2">
+        <f t="shared" ref="AD2:BF2" si="0">+AC2+1</f>
+        <v>2012</v>
+      </c>
+      <c r="AE2">
+        <f t="shared" si="0"/>
+        <v>2013</v>
+      </c>
+      <c r="AF2">
+        <f t="shared" si="0"/>
+        <v>2014</v>
+      </c>
+      <c r="AG2">
+        <f t="shared" si="0"/>
+        <v>2015</v>
+      </c>
+      <c r="AH2">
+        <f t="shared" si="0"/>
+        <v>2016</v>
+      </c>
+      <c r="AI2">
+        <f t="shared" si="0"/>
+        <v>2017</v>
+      </c>
+      <c r="AJ2">
+        <f t="shared" si="0"/>
+        <v>2018</v>
+      </c>
+      <c r="AK2">
+        <f t="shared" si="0"/>
+        <v>2019</v>
+      </c>
+      <c r="AL2">
+        <f t="shared" si="0"/>
+        <v>2020</v>
+      </c>
+      <c r="AM2">
+        <f t="shared" si="0"/>
+        <v>2021</v>
+      </c>
+      <c r="AN2">
+        <f t="shared" si="0"/>
+        <v>2022</v>
+      </c>
+      <c r="AO2">
+        <f t="shared" si="0"/>
+        <v>2023</v>
+      </c>
+      <c r="AP2">
+        <f t="shared" si="0"/>
+        <v>2024</v>
+      </c>
+      <c r="AQ2">
+        <f t="shared" si="0"/>
+        <v>2025</v>
+      </c>
+      <c r="AR2">
+        <f t="shared" si="0"/>
+        <v>2026</v>
+      </c>
+      <c r="AS2">
+        <f t="shared" si="0"/>
+        <v>2027</v>
+      </c>
+      <c r="AT2">
+        <f t="shared" si="0"/>
+        <v>2028</v>
+      </c>
+      <c r="AU2">
+        <f t="shared" si="0"/>
+        <v>2029</v>
+      </c>
+      <c r="AV2">
+        <f t="shared" si="0"/>
+        <v>2030</v>
+      </c>
+      <c r="AW2">
+        <f t="shared" si="0"/>
+        <v>2031</v>
+      </c>
+      <c r="AX2">
+        <f t="shared" si="0"/>
+        <v>2032</v>
+      </c>
+      <c r="AY2">
+        <f t="shared" si="0"/>
+        <v>2033</v>
+      </c>
+      <c r="AZ2">
+        <f t="shared" si="0"/>
+        <v>2034</v>
+      </c>
+      <c r="BA2">
+        <f t="shared" si="0"/>
+        <v>2035</v>
+      </c>
+      <c r="BB2">
+        <f t="shared" si="0"/>
+        <v>2036</v>
+      </c>
+      <c r="BC2">
+        <f t="shared" si="0"/>
+        <v>2037</v>
+      </c>
+      <c r="BD2">
+        <f t="shared" si="0"/>
+        <v>2038</v>
+      </c>
+      <c r="BE2">
+        <f t="shared" si="0"/>
+        <v>2039</v>
+      </c>
+      <c r="BF2">
+        <f t="shared" si="0"/>
+        <v>2040</v>
+      </c>
+    </row>
+    <row r="3" spans="1:58" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B3" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="G3" s="2">
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3">
         <v>7968</v>
       </c>
-      <c r="J3" s="2">
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3">
         <v>7389</v>
       </c>
-      <c r="K3" s="2">
+      <c r="K3" s="3">
         <v>7277</v>
       </c>
-    </row>
-    <row r="5" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
+      <c r="N3" s="3"/>
+    </row>
+    <row r="5" spans="1:58" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B5" s="1" t="s">
         <v>22</v>
       </c>
@@ -810,19 +1104,81 @@
       <c r="G5" s="3">
         <v>18094</v>
       </c>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
+      <c r="H5" s="3">
+        <v>20828</v>
+      </c>
+      <c r="I5" s="3">
+        <v>21050</v>
+      </c>
       <c r="J5" s="3">
         <v>20723</v>
       </c>
       <c r="K5" s="3">
         <v>16929</v>
       </c>
-      <c r="L5" s="3"/>
-      <c r="M5" s="3"/>
-      <c r="N5" s="3"/>
-    </row>
-    <row r="6" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="L5" s="1">
+        <v>18268</v>
+      </c>
+      <c r="M5" s="1">
+        <v>19943</v>
+      </c>
+      <c r="N5" s="1">
+        <v>19571</v>
+      </c>
+      <c r="O5" s="1">
+        <v>17972</v>
+      </c>
+      <c r="P5" s="1">
+        <v>21081</v>
+      </c>
+      <c r="Q5" s="1">
+        <v>21346</v>
+      </c>
+      <c r="R5" s="1">
+        <v>20804</v>
+      </c>
+      <c r="S5" s="1">
+        <v>18490</v>
+      </c>
+      <c r="T5" s="1">
+        <v>20625</v>
+      </c>
+      <c r="U5" s="1">
+        <f>+Q5</f>
+        <v>21346</v>
+      </c>
+      <c r="V5" s="1">
+        <f>+R5</f>
+        <v>20804</v>
+      </c>
+      <c r="AJ5" s="1">
+        <v>81912</v>
+      </c>
+      <c r="AK5" s="1">
+        <v>78093</v>
+      </c>
+      <c r="AL5" s="1">
+        <f>SUM(F5:I5)</f>
+        <v>59972</v>
+      </c>
+      <c r="AM5" s="1">
+        <f>SUM(G5:J5)</f>
+        <v>80695</v>
+      </c>
+      <c r="AN5" s="1">
+        <f>SUM(K5:N5)</f>
+        <v>74711</v>
+      </c>
+      <c r="AO5" s="1">
+        <f>SUM(O5:R5)</f>
+        <v>81203</v>
+      </c>
+      <c r="AP5" s="1">
+        <f>SUM(S5:V5)</f>
+        <v>81265</v>
+      </c>
+    </row>
+    <row r="6" spans="1:58" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
         <v>23</v>
       </c>
@@ -833,19 +1189,81 @@
       <c r="G6" s="3">
         <v>10040</v>
       </c>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
+      <c r="H6" s="3">
+        <v>10522</v>
+      </c>
+      <c r="I6" s="3">
+        <v>10871</v>
+      </c>
       <c r="J6" s="3">
         <v>12365</v>
       </c>
       <c r="K6" s="3">
         <v>11482</v>
       </c>
-      <c r="L6" s="3"/>
-      <c r="M6" s="3"/>
-      <c r="N6" s="3"/>
-    </row>
-    <row r="7" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="L6" s="1">
+        <v>11379</v>
+      </c>
+      <c r="M6" s="1">
+        <v>12597</v>
+      </c>
+      <c r="N6" s="1">
+        <v>13506</v>
+      </c>
+      <c r="O6" s="1">
+        <v>13172</v>
+      </c>
+      <c r="P6" s="1">
+        <v>12975</v>
+      </c>
+      <c r="Q6" s="1">
+        <v>13101</v>
+      </c>
+      <c r="R6" s="1">
+        <v>14147</v>
+      </c>
+      <c r="S6" s="1">
+        <v>13023</v>
+      </c>
+      <c r="T6" s="1">
+        <v>13306</v>
+      </c>
+      <c r="U6" s="1">
+        <f>+Q6</f>
+        <v>13101</v>
+      </c>
+      <c r="V6" s="1">
+        <f>+R6</f>
+        <v>14147</v>
+      </c>
+      <c r="AJ6" s="1">
+        <v>20365</v>
+      </c>
+      <c r="AK6" s="1">
+        <v>29320</v>
+      </c>
+      <c r="AL6" s="1">
+        <f>SUM(F6:I6)</f>
+        <v>31433</v>
+      </c>
+      <c r="AM6" s="1">
+        <f>SUM(G6:J6)</f>
+        <v>43798</v>
+      </c>
+      <c r="AN6" s="1">
+        <f>SUM(K6:N6)</f>
+        <v>48964</v>
+      </c>
+      <c r="AO6" s="1">
+        <f>SUM(O6:R6)</f>
+        <v>53395</v>
+      </c>
+      <c r="AP6" s="1">
+        <f>SUM(S6:V6)</f>
+        <v>53577</v>
+      </c>
+    </row>
+    <row r="7" spans="1:58" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B7" s="4" t="s">
         <v>10</v>
       </c>
@@ -857,8 +1275,14 @@
         <f>+G5+G6</f>
         <v>28134</v>
       </c>
-      <c r="H7" s="5"/>
-      <c r="I7" s="5"/>
+      <c r="H7" s="5">
+        <f>+H5+H6</f>
+        <v>31350</v>
+      </c>
+      <c r="I7" s="5">
+        <f>+I5+I6</f>
+        <v>31921</v>
+      </c>
       <c r="J7" s="5">
         <f>+J5+J6</f>
         <v>33088</v>
@@ -867,11 +1291,80 @@
         <f>+K5+K6</f>
         <v>28411</v>
       </c>
-      <c r="L7" s="5"/>
-      <c r="M7" s="5"/>
-      <c r="N7" s="5"/>
-    </row>
-    <row r="8" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="L7" s="4">
+        <f>+L5+L6</f>
+        <v>29647</v>
+      </c>
+      <c r="M7" s="4">
+        <f>+M5+M6</f>
+        <v>32540</v>
+      </c>
+      <c r="N7" s="4">
+        <f>+N5+N6</f>
+        <v>33077</v>
+      </c>
+      <c r="O7" s="4">
+        <f>+O5+O6</f>
+        <v>31144</v>
+      </c>
+      <c r="P7" s="4">
+        <f>+P5+P6</f>
+        <v>34056</v>
+      </c>
+      <c r="Q7" s="4">
+        <f>+Q5+Q6</f>
+        <v>34447</v>
+      </c>
+      <c r="R7" s="4">
+        <f>+R5+R6</f>
+        <v>34951</v>
+      </c>
+      <c r="S7" s="4">
+        <f>+S5+S6</f>
+        <v>31513</v>
+      </c>
+      <c r="T7" s="4">
+        <f>+T5+T6</f>
+        <v>33931</v>
+      </c>
+      <c r="U7" s="4">
+        <f>+U5+U6</f>
+        <v>34447</v>
+      </c>
+      <c r="V7" s="4">
+        <f>+V5+V6</f>
+        <v>34951</v>
+      </c>
+      <c r="AJ7" s="4">
+        <f t="shared" ref="AJ7:AK7" si="1">+AJ5+AJ6</f>
+        <v>102277</v>
+      </c>
+      <c r="AK7" s="4">
+        <f t="shared" si="1"/>
+        <v>107413</v>
+      </c>
+      <c r="AL7" s="4">
+        <f>+AL5+AL6</f>
+        <v>91405</v>
+      </c>
+      <c r="AM7" s="4">
+        <f>+AM5+AM6</f>
+        <v>124493</v>
+      </c>
+      <c r="AN7" s="4">
+        <f>+AN5+AN6</f>
+        <v>123675</v>
+      </c>
+      <c r="AO7" s="4">
+        <f>+AO5+AO6</f>
+        <v>134598</v>
+      </c>
+      <c r="AP7" s="4">
+        <f>+AP6+AP5</f>
+        <v>134842</v>
+      </c>
+    </row>
+    <row r="8" spans="1:58" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
         <v>24</v>
       </c>
@@ -882,19 +1375,81 @@
       <c r="G8" s="3">
         <v>15002</v>
       </c>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
+      <c r="H8" s="3">
+        <v>15897</v>
+      </c>
+      <c r="I8" s="3">
+        <v>16126</v>
+      </c>
       <c r="J8" s="3">
         <v>17289</v>
       </c>
       <c r="K8" s="3">
         <v>15546</v>
       </c>
-      <c r="L8" s="3"/>
-      <c r="M8" s="3"/>
-      <c r="N8" s="3"/>
-    </row>
-    <row r="9" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="L8" s="1">
+        <v>15171</v>
+      </c>
+      <c r="M8" s="1">
+        <v>16273</v>
+      </c>
+      <c r="N8" s="1">
+        <v>16945</v>
+      </c>
+      <c r="O8" s="1">
+        <v>15152</v>
+      </c>
+      <c r="P8" s="1">
+        <v>16167</v>
+      </c>
+      <c r="Q8" s="1">
+        <v>16294</v>
+      </c>
+      <c r="R8" s="1">
+        <v>17418</v>
+      </c>
+      <c r="S8" s="1">
+        <v>15291</v>
+      </c>
+      <c r="T8" s="1">
+        <v>16398</v>
+      </c>
+      <c r="U8" s="1">
+        <f>+U7-U9</f>
+        <v>16534.559999999998</v>
+      </c>
+      <c r="V8" s="1">
+        <f>+V7-V9</f>
+        <v>16776.48</v>
+      </c>
+      <c r="AJ8" s="1">
+        <v>51744</v>
+      </c>
+      <c r="AK8" s="1">
+        <v>62850</v>
+      </c>
+      <c r="AL8" s="1">
+        <f>SUM(F8:I8)</f>
+        <v>47025</v>
+      </c>
+      <c r="AM8" s="1">
+        <f>SUM(G8:J8)</f>
+        <v>64314</v>
+      </c>
+      <c r="AN8" s="1">
+        <f>SUM(K8:N8)</f>
+        <v>63935</v>
+      </c>
+      <c r="AO8" s="1">
+        <f>SUM(O8:R8)</f>
+        <v>65031</v>
+      </c>
+      <c r="AP8" s="1">
+        <f>SUM(S8:V8)</f>
+        <v>65000.039999999994</v>
+      </c>
+    </row>
+    <row r="9" spans="1:58" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
         <v>25</v>
       </c>
@@ -906,21 +1461,96 @@
         <f>+G7-G8</f>
         <v>13132</v>
       </c>
-      <c r="H9" s="3"/>
-      <c r="I9" s="3"/>
+      <c r="H9" s="3">
+        <f t="shared" ref="H9:I9" si="2">+H7-H8</f>
+        <v>15453</v>
+      </c>
+      <c r="I9" s="3">
+        <f t="shared" si="2"/>
+        <v>15795</v>
+      </c>
       <c r="J9" s="3">
-        <f t="shared" ref="J9:K9" si="0">+J7-J8</f>
+        <f t="shared" ref="J9:K9" si="3">+J7-J8</f>
         <v>15799</v>
       </c>
       <c r="K9" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>12865</v>
       </c>
-      <c r="L9" s="3"/>
-      <c r="M9" s="3"/>
-      <c r="N9" s="3"/>
-    </row>
-    <row r="10" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="L9" s="1">
+        <f>+L7-L8</f>
+        <v>14476</v>
+      </c>
+      <c r="M9" s="1">
+        <f>+M7-M8</f>
+        <v>16267</v>
+      </c>
+      <c r="N9" s="1">
+        <f>+N7-N8</f>
+        <v>16132</v>
+      </c>
+      <c r="O9" s="1">
+        <f>+O7-O8</f>
+        <v>15992</v>
+      </c>
+      <c r="P9" s="1">
+        <f>+P7-P8</f>
+        <v>17889</v>
+      </c>
+      <c r="Q9" s="1">
+        <f>+Q7-Q8</f>
+        <v>18153</v>
+      </c>
+      <c r="R9" s="1">
+        <f>+R7-R8</f>
+        <v>17533</v>
+      </c>
+      <c r="S9" s="1">
+        <f>+S7-S8</f>
+        <v>16222</v>
+      </c>
+      <c r="T9" s="1">
+        <f>+T7-T8</f>
+        <v>17533</v>
+      </c>
+      <c r="U9" s="1">
+        <f>+U7*0.52</f>
+        <v>17912.440000000002</v>
+      </c>
+      <c r="V9" s="1">
+        <f>+V7*0.52</f>
+        <v>18174.52</v>
+      </c>
+      <c r="AJ9" s="1">
+        <f t="shared" ref="AJ9:AK9" si="4">+AJ7-AJ8</f>
+        <v>50533</v>
+      </c>
+      <c r="AK9" s="1">
+        <f t="shared" si="4"/>
+        <v>44563</v>
+      </c>
+      <c r="AL9" s="1">
+        <f>+AL7-AL8</f>
+        <v>44380</v>
+      </c>
+      <c r="AM9" s="1">
+        <f>+AM7-AM8</f>
+        <v>60179</v>
+      </c>
+      <c r="AN9" s="1">
+        <f>+AN7-AN8</f>
+        <v>59740</v>
+      </c>
+      <c r="AO9" s="1">
+        <f>+AO7-AO8</f>
+        <v>69567</v>
+      </c>
+      <c r="AP9" s="1">
+        <f>+AP7-AP8</f>
+        <v>69841.960000000006</v>
+      </c>
+    </row>
+    <row r="10" spans="1:58" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
         <v>26</v>
       </c>
@@ -931,19 +1561,81 @@
       <c r="G10" s="3">
         <v>5245</v>
       </c>
-      <c r="H10" s="3"/>
-      <c r="I10" s="3"/>
+      <c r="H10" s="3">
+        <v>5707</v>
+      </c>
+      <c r="I10" s="3">
+        <v>7320</v>
+      </c>
       <c r="J10" s="3">
         <v>6451</v>
       </c>
       <c r="K10" s="3">
         <v>4656</v>
       </c>
-      <c r="L10" s="3"/>
-      <c r="M10" s="3"/>
-      <c r="N10" s="3"/>
-    </row>
-    <row r="11" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="L10" s="1">
+        <v>4784</v>
+      </c>
+      <c r="M10" s="1">
+        <v>5193</v>
+      </c>
+      <c r="N10" s="1">
+        <v>5881</v>
+      </c>
+      <c r="O10" s="1">
+        <v>5589</v>
+      </c>
+      <c r="P10" s="1">
+        <v>6298</v>
+      </c>
+      <c r="Q10" s="1">
+        <v>5778</v>
+      </c>
+      <c r="R10" s="1">
+        <v>5854</v>
+      </c>
+      <c r="S10" s="1">
+        <v>5375</v>
+      </c>
+      <c r="T10" s="1">
+        <v>5700</v>
+      </c>
+      <c r="U10" s="1">
+        <f>+Q10</f>
+        <v>5778</v>
+      </c>
+      <c r="V10" s="1">
+        <f>+R10</f>
+        <v>5854</v>
+      </c>
+      <c r="AJ10" s="1">
+        <v>19231</v>
+      </c>
+      <c r="AK10" s="1">
+        <v>19910</v>
+      </c>
+      <c r="AL10" s="1">
+        <f>SUM(F10:I10)</f>
+        <v>18272</v>
+      </c>
+      <c r="AM10" s="1">
+        <f>SUM(G10:J10)</f>
+        <v>24723</v>
+      </c>
+      <c r="AN10" s="1">
+        <f>SUM(K10:N10)</f>
+        <v>20514</v>
+      </c>
+      <c r="AO10" s="1">
+        <f>SUM(O10:R10)</f>
+        <v>23519</v>
+      </c>
+      <c r="AP10" s="1">
+        <f>SUM(S10:V10)</f>
+        <v>22707</v>
+      </c>
+    </row>
+    <row r="11" spans="1:58" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
         <v>27</v>
       </c>
@@ -954,19 +1646,81 @@
       <c r="G11" s="3">
         <v>5098</v>
       </c>
-      <c r="H11" s="3"/>
-      <c r="I11" s="3"/>
+      <c r="H11" s="3">
+        <v>6283</v>
+      </c>
+      <c r="I11" s="3">
+        <v>6167</v>
+      </c>
       <c r="J11" s="3">
         <v>7390</v>
       </c>
       <c r="K11" s="3">
         <v>5608</v>
       </c>
-      <c r="L11" s="3"/>
-      <c r="M11" s="3"/>
-      <c r="N11" s="3"/>
-    </row>
-    <row r="12" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="L11" s="1">
+        <v>6292</v>
+      </c>
+      <c r="M11" s="1">
+        <v>5757</v>
+      </c>
+      <c r="N11" s="1">
+        <v>5658</v>
+      </c>
+      <c r="O11" s="1">
+        <v>5423</v>
+      </c>
+      <c r="P11" s="1">
+        <v>6381</v>
+      </c>
+      <c r="Q11" s="1">
+        <v>6101</v>
+      </c>
+      <c r="R11" s="1">
+        <v>6287</v>
+      </c>
+      <c r="S11" s="1">
+        <v>5363</v>
+      </c>
+      <c r="T11" s="1">
+        <v>5889</v>
+      </c>
+      <c r="U11" s="1">
+        <f>+Q11</f>
+        <v>6101</v>
+      </c>
+      <c r="V11" s="1">
+        <f>+R11</f>
+        <v>6287</v>
+      </c>
+      <c r="AJ11" s="1">
+        <v>15772</v>
+      </c>
+      <c r="AK11" s="1">
+        <v>18346</v>
+      </c>
+      <c r="AL11" s="1">
+        <f>SUM(F11:I11)</f>
+        <v>17548</v>
+      </c>
+      <c r="AM11" s="1">
+        <f>SUM(G11:J11)</f>
+        <v>24938</v>
+      </c>
+      <c r="AN11" s="1">
+        <f>SUM(K11:N11)</f>
+        <v>23315</v>
+      </c>
+      <c r="AO11" s="1">
+        <f>SUM(O11:R11)</f>
+        <v>24192</v>
+      </c>
+      <c r="AP11" s="1">
+        <f>SUM(S11:V11)</f>
+        <v>23640</v>
+      </c>
+    </row>
+    <row r="12" spans="1:58" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
         <v>28</v>
       </c>
@@ -978,8 +1732,14 @@
         <f>+G10+G11</f>
         <v>10343</v>
       </c>
-      <c r="H12" s="3"/>
-      <c r="I12" s="3"/>
+      <c r="H12" s="3">
+        <f>+H10+H11</f>
+        <v>11990</v>
+      </c>
+      <c r="I12" s="3">
+        <f>+I10+I11</f>
+        <v>13487</v>
+      </c>
       <c r="J12" s="3">
         <f>+J10+J11</f>
         <v>13841</v>
@@ -988,11 +1748,80 @@
         <f>+K10+K11</f>
         <v>10264</v>
       </c>
-      <c r="L12" s="3"/>
-      <c r="M12" s="3"/>
-      <c r="N12" s="3"/>
-    </row>
-    <row r="13" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="L12" s="3">
+        <f t="shared" ref="L12:P12" si="5">+L10+L11</f>
+        <v>11076</v>
+      </c>
+      <c r="M12" s="3">
+        <f t="shared" si="5"/>
+        <v>10950</v>
+      </c>
+      <c r="N12" s="3">
+        <f t="shared" si="5"/>
+        <v>11539</v>
+      </c>
+      <c r="O12" s="3">
+        <f t="shared" si="5"/>
+        <v>11012</v>
+      </c>
+      <c r="P12" s="3">
+        <f t="shared" si="5"/>
+        <v>12679</v>
+      </c>
+      <c r="Q12" s="3">
+        <f t="shared" ref="Q12:R12" si="6">+Q10+Q11</f>
+        <v>11879</v>
+      </c>
+      <c r="R12" s="3">
+        <f t="shared" si="6"/>
+        <v>12141</v>
+      </c>
+      <c r="S12" s="3">
+        <f t="shared" ref="S12" si="7">+S10+S11</f>
+        <v>10738</v>
+      </c>
+      <c r="T12" s="3">
+        <f>+T10+T11</f>
+        <v>11589</v>
+      </c>
+      <c r="U12" s="3">
+        <f>+U10+U11</f>
+        <v>11879</v>
+      </c>
+      <c r="V12" s="3">
+        <f>+V10+V11</f>
+        <v>12141</v>
+      </c>
+      <c r="AJ12" s="1">
+        <f t="shared" ref="AJ12:AK12" si="8">+AJ11+AJ10</f>
+        <v>35003</v>
+      </c>
+      <c r="AK12" s="1">
+        <f t="shared" si="8"/>
+        <v>38256</v>
+      </c>
+      <c r="AL12" s="1">
+        <f>+AL11+AL10</f>
+        <v>35820</v>
+      </c>
+      <c r="AM12" s="1">
+        <f>+AM11+AM10</f>
+        <v>49661</v>
+      </c>
+      <c r="AN12" s="1">
+        <f t="shared" ref="AN12:AP12" si="9">+AN11+AN10</f>
+        <v>43829</v>
+      </c>
+      <c r="AO12" s="1">
+        <f t="shared" si="9"/>
+        <v>47711</v>
+      </c>
+      <c r="AP12" s="1">
+        <f t="shared" si="9"/>
+        <v>46347</v>
+      </c>
+    </row>
+    <row r="13" spans="1:58" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
         <v>29</v>
       </c>
@@ -1004,8 +1833,14 @@
         <f>+G9-G12</f>
         <v>2789</v>
       </c>
-      <c r="H13" s="3"/>
-      <c r="I13" s="3"/>
+      <c r="H13" s="3">
+        <f>+H9-H12</f>
+        <v>3463</v>
+      </c>
+      <c r="I13" s="3">
+        <f>+I9-I12</f>
+        <v>2308</v>
+      </c>
       <c r="J13" s="3">
         <f>+J9-J12</f>
         <v>1958</v>
@@ -1014,11 +1849,80 @@
         <f>+K9-K12</f>
         <v>2601</v>
       </c>
-      <c r="L13" s="3"/>
-      <c r="M13" s="3"/>
-      <c r="N13" s="3"/>
-    </row>
-    <row r="14" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="L13" s="3">
+        <f t="shared" ref="L13:P13" si="10">+L9-L12</f>
+        <v>3400</v>
+      </c>
+      <c r="M13" s="3">
+        <f t="shared" si="10"/>
+        <v>5317</v>
+      </c>
+      <c r="N13" s="3">
+        <f t="shared" si="10"/>
+        <v>4593</v>
+      </c>
+      <c r="O13" s="3">
+        <f t="shared" si="10"/>
+        <v>4980</v>
+      </c>
+      <c r="P13" s="3">
+        <f t="shared" si="10"/>
+        <v>5210</v>
+      </c>
+      <c r="Q13" s="3">
+        <f t="shared" ref="Q13:R13" si="11">+Q9-Q12</f>
+        <v>6274</v>
+      </c>
+      <c r="R13" s="3">
+        <f t="shared" si="11"/>
+        <v>5392</v>
+      </c>
+      <c r="S13" s="3">
+        <f t="shared" ref="S13" si="12">+S9-S12</f>
+        <v>5484</v>
+      </c>
+      <c r="T13" s="3">
+        <f>+T9-T12</f>
+        <v>5944</v>
+      </c>
+      <c r="U13" s="3">
+        <f>+U9-U12</f>
+        <v>6033.4400000000023</v>
+      </c>
+      <c r="V13" s="3">
+        <f>+V9-V12</f>
+        <v>6033.52</v>
+      </c>
+      <c r="AJ13" s="1">
+        <f t="shared" ref="AJ13:AK13" si="13">+AJ9-AJ12</f>
+        <v>15530</v>
+      </c>
+      <c r="AK13" s="1">
+        <f t="shared" si="13"/>
+        <v>6307</v>
+      </c>
+      <c r="AL13" s="1">
+        <f>+AL9-AL12</f>
+        <v>8560</v>
+      </c>
+      <c r="AM13" s="1">
+        <f>+AM9-AM12</f>
+        <v>10518</v>
+      </c>
+      <c r="AN13" s="1">
+        <f t="shared" ref="AN13:AP13" si="14">+AN9-AN12</f>
+        <v>15911</v>
+      </c>
+      <c r="AO13" s="1">
+        <f t="shared" si="14"/>
+        <v>21856</v>
+      </c>
+      <c r="AP13" s="1">
+        <f t="shared" si="14"/>
+        <v>23494.960000000006</v>
+      </c>
+    </row>
+    <row r="14" spans="1:58" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B14" s="1" t="s">
         <v>30</v>
       </c>
@@ -1030,8 +1934,14 @@
         <f>1233-823</f>
         <v>410</v>
       </c>
-      <c r="H14" s="3"/>
-      <c r="I14" s="3"/>
+      <c r="H14" s="3">
+        <f>1342-845-36-4</f>
+        <v>457</v>
+      </c>
+      <c r="I14" s="3">
+        <f>1462-880+7-4</f>
+        <v>585</v>
+      </c>
       <c r="J14" s="3">
         <f>1514-873</f>
         <v>641</v>
@@ -1040,11 +1950,70 @@
         <f>1454-710</f>
         <v>744</v>
       </c>
-      <c r="L14" s="3"/>
-      <c r="M14" s="3"/>
-      <c r="N14" s="3"/>
-    </row>
-    <row r="15" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="L14" s="1">
+        <v>151</v>
+      </c>
+      <c r="M14" s="1">
+        <v>-4770</v>
+      </c>
+      <c r="N14" s="1">
+        <v>1781</v>
+      </c>
+      <c r="O14" s="1">
+        <v>2595</v>
+      </c>
+      <c r="P14" s="1">
+        <v>1369</v>
+      </c>
+      <c r="Q14" s="1">
+        <v>1905</v>
+      </c>
+      <c r="R14" s="1">
+        <v>-2527</v>
+      </c>
+      <c r="S14" s="1">
+        <v>1246</v>
+      </c>
+      <c r="T14" s="1">
+        <f>1993-742+93-119-454</f>
+        <v>771</v>
+      </c>
+      <c r="U14" s="1">
+        <f>+Q14</f>
+        <v>1905</v>
+      </c>
+      <c r="V14" s="1">
+        <f>+R14</f>
+        <v>-2527</v>
+      </c>
+      <c r="AJ14" s="1">
+        <v>11795</v>
+      </c>
+      <c r="AK14" s="1">
+        <v>-6647</v>
+      </c>
+      <c r="AL14" s="1">
+        <f>SUM(F14:I14)</f>
+        <v>1452</v>
+      </c>
+      <c r="AM14" s="1">
+        <f>SUM(G14:J14)</f>
+        <v>2093</v>
+      </c>
+      <c r="AN14" s="1">
+        <f>SUM(K14:N14)</f>
+        <v>-2094</v>
+      </c>
+      <c r="AO14" s="1">
+        <f>SUM(O14:R14)</f>
+        <v>3342</v>
+      </c>
+      <c r="AP14" s="1">
+        <f>SUM(S14:V14)</f>
+        <v>1395</v>
+      </c>
+    </row>
+    <row r="15" spans="1:58" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
         <v>31</v>
       </c>
@@ -1056,8 +2025,14 @@
         <f>+G13+G14</f>
         <v>3199</v>
       </c>
-      <c r="H15" s="3"/>
-      <c r="I15" s="3"/>
+      <c r="H15" s="3">
+        <f>+H13+H14</f>
+        <v>3920</v>
+      </c>
+      <c r="I15" s="3">
+        <f>+I13+I14</f>
+        <v>2893</v>
+      </c>
       <c r="J15" s="3">
         <f>+J13+J14</f>
         <v>2599</v>
@@ -1066,11 +2041,80 @@
         <f>+K13+K14</f>
         <v>3345</v>
       </c>
-      <c r="L15" s="3"/>
-      <c r="M15" s="3"/>
-      <c r="N15" s="3"/>
-    </row>
-    <row r="16" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="L15" s="3">
+        <f t="shared" ref="L15:V15" si="15">+L13+L14</f>
+        <v>3551</v>
+      </c>
+      <c r="M15" s="3">
+        <f t="shared" si="15"/>
+        <v>547</v>
+      </c>
+      <c r="N15" s="3">
+        <f t="shared" si="15"/>
+        <v>6374</v>
+      </c>
+      <c r="O15" s="3">
+        <f t="shared" si="15"/>
+        <v>7575</v>
+      </c>
+      <c r="P15" s="3">
+        <f t="shared" si="15"/>
+        <v>6579</v>
+      </c>
+      <c r="Q15" s="3">
+        <f t="shared" si="15"/>
+        <v>8179</v>
+      </c>
+      <c r="R15" s="3">
+        <f t="shared" si="15"/>
+        <v>2865</v>
+      </c>
+      <c r="S15" s="3">
+        <f t="shared" si="15"/>
+        <v>6730</v>
+      </c>
+      <c r="T15" s="3">
+        <f t="shared" si="15"/>
+        <v>6715</v>
+      </c>
+      <c r="U15" s="3">
+        <f t="shared" si="15"/>
+        <v>7938.4400000000023</v>
+      </c>
+      <c r="V15" s="3">
+        <f t="shared" si="15"/>
+        <v>3506.5200000000004</v>
+      </c>
+      <c r="AJ15" s="1">
+        <f t="shared" ref="AJ15:AK15" si="16">+AJ13+AJ14</f>
+        <v>27325</v>
+      </c>
+      <c r="AK15" s="1">
+        <f t="shared" si="16"/>
+        <v>-340</v>
+      </c>
+      <c r="AL15" s="1">
+        <f>+AL13+AL14</f>
+        <v>10012</v>
+      </c>
+      <c r="AM15" s="1">
+        <f>+AM13+AM14</f>
+        <v>12611</v>
+      </c>
+      <c r="AN15" s="1">
+        <f>+AN13+AN14</f>
+        <v>13817</v>
+      </c>
+      <c r="AO15" s="1">
+        <f>+AO13+AO14</f>
+        <v>25198</v>
+      </c>
+      <c r="AP15" s="1">
+        <f>+AP13+AP14</f>
+        <v>24889.960000000006</v>
+      </c>
+    </row>
+    <row r="16" spans="1:58" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B16" s="1" t="s">
         <v>32</v>
       </c>
@@ -1082,8 +2126,13 @@
         <f>1534-621</f>
         <v>913</v>
       </c>
-      <c r="H16" s="3"/>
-      <c r="I16" s="3"/>
+      <c r="H16" s="3">
+        <f>1618-246</f>
+        <v>1372</v>
+      </c>
+      <c r="I16" s="3">
+        <v>0</v>
+      </c>
       <c r="J16" s="3">
         <f>1295-645</f>
         <v>650</v>
@@ -1092,11 +2141,78 @@
         <f>391+134</f>
         <v>525</v>
       </c>
-      <c r="L16" s="3"/>
-      <c r="M16" s="3"/>
-      <c r="N16" s="3"/>
-    </row>
-    <row r="17" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="L16" s="1">
+        <f>25-111</f>
+        <v>-86</v>
+      </c>
+      <c r="M16" s="1">
+        <f>908-215</f>
+        <v>693</v>
+      </c>
+      <c r="N16" s="1">
+        <f>1254+167</f>
+        <v>1421</v>
+      </c>
+      <c r="O16" s="1">
+        <f>1193+557</f>
+        <v>1750</v>
+      </c>
+      <c r="P16" s="1">
+        <f>1270+99</f>
+        <v>1369</v>
+      </c>
+      <c r="Q16" s="1">
+        <f>1282+216</f>
+        <v>1498</v>
+      </c>
+      <c r="R16" s="1">
+        <f>-96+362</f>
+        <v>266</v>
+      </c>
+      <c r="S16" s="1">
+        <f>883+399</f>
+        <v>1282</v>
+      </c>
+      <c r="T16" s="1">
+        <f>1270+99</f>
+        <v>1369</v>
+      </c>
+      <c r="U16" s="1">
+        <f>+Q16</f>
+        <v>1498</v>
+      </c>
+      <c r="V16" s="1">
+        <f>+R16</f>
+        <v>266</v>
+      </c>
+      <c r="AJ16" s="1">
+        <v>4743</v>
+      </c>
+      <c r="AK16" s="1">
+        <v>1948</v>
+      </c>
+      <c r="AL16" s="1">
+        <f>SUM(F16:I16)</f>
+        <v>2285</v>
+      </c>
+      <c r="AM16" s="1">
+        <f>SUM(G16:J16)</f>
+        <v>2935</v>
+      </c>
+      <c r="AN16" s="1">
+        <f>SUM(K16:N16)</f>
+        <v>2553</v>
+      </c>
+      <c r="AO16" s="1">
+        <f>SUM(O16:R16)</f>
+        <v>4883</v>
+      </c>
+      <c r="AP16" s="1">
+        <f>SUM(S16:V16)</f>
+        <v>4415</v>
+      </c>
+    </row>
+    <row r="17" spans="2:42" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B17" s="1" t="s">
         <v>33</v>
       </c>
@@ -1108,8 +2224,14 @@
         <f>+G15-G16</f>
         <v>2286</v>
       </c>
-      <c r="H17" s="3"/>
-      <c r="I17" s="3"/>
+      <c r="H17" s="3">
+        <f>+H15-H16</f>
+        <v>2548</v>
+      </c>
+      <c r="I17" s="3">
+        <f>+I15-I16</f>
+        <v>2893</v>
+      </c>
       <c r="J17" s="3">
         <f>+J15-J16</f>
         <v>1949</v>
@@ -1118,11 +2240,80 @@
         <f>+K15-K16</f>
         <v>2820</v>
       </c>
-      <c r="L17" s="3"/>
-      <c r="M17" s="3"/>
-      <c r="N17" s="3"/>
-    </row>
-    <row r="18" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="L17" s="3">
+        <f t="shared" ref="L17:V17" si="17">+L15-L16</f>
+        <v>3637</v>
+      </c>
+      <c r="M17" s="3">
+        <f t="shared" si="17"/>
+        <v>-146</v>
+      </c>
+      <c r="N17" s="3">
+        <f t="shared" si="17"/>
+        <v>4953</v>
+      </c>
+      <c r="O17" s="3">
+        <f t="shared" si="17"/>
+        <v>5825</v>
+      </c>
+      <c r="P17" s="3">
+        <f t="shared" si="17"/>
+        <v>5210</v>
+      </c>
+      <c r="Q17" s="3">
+        <f t="shared" si="17"/>
+        <v>6681</v>
+      </c>
+      <c r="R17" s="3">
+        <f t="shared" si="17"/>
+        <v>2599</v>
+      </c>
+      <c r="S17" s="3">
+        <f t="shared" si="17"/>
+        <v>5448</v>
+      </c>
+      <c r="T17" s="3">
+        <f t="shared" si="17"/>
+        <v>5346</v>
+      </c>
+      <c r="U17" s="3">
+        <f t="shared" si="17"/>
+        <v>6440.4400000000023</v>
+      </c>
+      <c r="V17" s="3">
+        <f t="shared" si="17"/>
+        <v>3240.5200000000004</v>
+      </c>
+      <c r="AJ17" s="1">
+        <f t="shared" ref="AJ17:AK17" si="18">+AJ15-AJ16</f>
+        <v>22582</v>
+      </c>
+      <c r="AK17" s="1">
+        <f t="shared" si="18"/>
+        <v>-2288</v>
+      </c>
+      <c r="AL17" s="1">
+        <f>+AL15-AL16</f>
+        <v>7727</v>
+      </c>
+      <c r="AM17" s="1">
+        <f>+AM15-AM16</f>
+        <v>9676</v>
+      </c>
+      <c r="AN17" s="1">
+        <f>+AN15-AN16</f>
+        <v>11264</v>
+      </c>
+      <c r="AO17" s="1">
+        <f>+AO15-AO16</f>
+        <v>20315</v>
+      </c>
+      <c r="AP17" s="1">
+        <f>+AP15-AP16</f>
+        <v>20474.960000000006</v>
+      </c>
+    </row>
+    <row r="18" spans="2:42" x14ac:dyDescent="0.2">
       <c r="B18" s="1" t="s">
         <v>34</v>
       </c>
@@ -1130,6 +2321,14 @@
         <f>+G17/G19</f>
         <v>0.82319049333813465</v>
       </c>
+      <c r="H18" s="6">
+        <f>+H17/H19</f>
+        <v>0.9275573352748453</v>
+      </c>
+      <c r="I18" s="6">
+        <f>+I17/I19</f>
+        <v>1.0413966882649388</v>
+      </c>
       <c r="J18" s="6">
         <f>+J17/J19</f>
         <v>0.69211647727272729</v>
@@ -1138,8 +2337,74 @@
         <f>+K17/K19</f>
         <v>1.0191543187567762</v>
       </c>
-    </row>
-    <row r="19" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="L18" s="6">
+        <f t="shared" ref="L18:V18" si="19">+L17/L19</f>
+        <v>1.2938456065457133</v>
+      </c>
+      <c r="M18" s="6">
+        <f t="shared" si="19"/>
+        <v>-5.2329749103942655E-2</v>
+      </c>
+      <c r="N18" s="6">
+        <f t="shared" si="19"/>
+        <v>1.7682970367725812</v>
+      </c>
+      <c r="O18" s="6">
+        <f t="shared" si="19"/>
+        <v>2.0532252379273879</v>
+      </c>
+      <c r="P18" s="6">
+        <f t="shared" si="19"/>
+        <v>1.8383909668313339</v>
+      </c>
+      <c r="Q18" s="6">
+        <f t="shared" si="19"/>
+        <v>2.3475052705551653</v>
+      </c>
+      <c r="R18" s="6">
+        <f t="shared" si="19"/>
+        <v>0.91837455830388692</v>
+      </c>
+      <c r="S18" s="6">
+        <f t="shared" si="19"/>
+        <v>1.9346590909090908</v>
+      </c>
+      <c r="T18" s="6">
+        <f t="shared" si="19"/>
+        <v>1.8863796753705011</v>
+      </c>
+      <c r="U18" s="6">
+        <f t="shared" si="19"/>
+        <v>2.2725617501764299</v>
+      </c>
+      <c r="V18" s="6">
+        <f t="shared" si="19"/>
+        <v>1.1434438955539874</v>
+      </c>
+      <c r="AJ18" s="10"/>
+      <c r="AK18" s="10"/>
+      <c r="AL18" s="10">
+        <f>+AL17/AL19</f>
+        <v>2.7922187424716935</v>
+      </c>
+      <c r="AM18" s="10">
+        <f t="shared" ref="AM18:AP18" si="20">+AM17/AM19</f>
+        <v>3.481201654973916</v>
+      </c>
+      <c r="AN18" s="10">
+        <f t="shared" si="20"/>
+        <v>4.034022741516698</v>
+      </c>
+      <c r="AO18" s="10">
+        <f t="shared" si="20"/>
+        <v>7.1613642372433244</v>
+      </c>
+      <c r="AP18" s="10">
+        <f t="shared" si="20"/>
+        <v>7.2362466866937645</v>
+      </c>
+    </row>
+    <row r="19" spans="2:42" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B19" s="1" t="s">
         <v>1</v>
       </c>
@@ -1150,19 +2415,212 @@
       <c r="G19" s="3">
         <v>2777</v>
       </c>
-      <c r="H19" s="3"/>
-      <c r="I19" s="3"/>
+      <c r="H19" s="3">
+        <v>2747</v>
+      </c>
+      <c r="I19" s="3">
+        <v>2778</v>
+      </c>
       <c r="J19" s="3">
         <v>2816</v>
       </c>
       <c r="K19" s="3">
         <v>2767</v>
       </c>
-      <c r="L19" s="3"/>
-      <c r="M19" s="3"/>
-      <c r="N19" s="3"/>
-    </row>
-    <row r="24" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="L19" s="1">
+        <v>2811</v>
+      </c>
+      <c r="M19" s="1">
+        <v>2790</v>
+      </c>
+      <c r="N19" s="1">
+        <v>2801</v>
+      </c>
+      <c r="O19" s="1">
+        <v>2837</v>
+      </c>
+      <c r="P19" s="1">
+        <v>2834</v>
+      </c>
+      <c r="Q19" s="1">
+        <v>2846</v>
+      </c>
+      <c r="R19" s="1">
+        <v>2830</v>
+      </c>
+      <c r="S19" s="1">
+        <v>2816</v>
+      </c>
+      <c r="T19" s="1">
+        <v>2834</v>
+      </c>
+      <c r="U19" s="1">
+        <f>+T19</f>
+        <v>2834</v>
+      </c>
+      <c r="V19" s="1">
+        <f>+U19</f>
+        <v>2834</v>
+      </c>
+      <c r="AL19" s="1">
+        <f>AVERAGE(F19:I19)</f>
+        <v>2767.3333333333335</v>
+      </c>
+      <c r="AM19" s="1">
+        <f>AVERAGE(G19:J19)</f>
+        <v>2779.5</v>
+      </c>
+      <c r="AN19" s="1">
+        <f>AVERAGE(K19:N19)</f>
+        <v>2792.25</v>
+      </c>
+      <c r="AO19" s="1">
+        <f>AVERAGE(O19:R19)</f>
+        <v>2836.75</v>
+      </c>
+      <c r="AP19" s="1">
+        <f>AVERAGE(S19:V19)</f>
+        <v>2829.5</v>
+      </c>
+    </row>
+    <row r="21" spans="2:42" x14ac:dyDescent="0.2">
+      <c r="B21" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="K21" s="8">
+        <f>+K7/G7-1</f>
+        <v>9.8457382526480064E-3</v>
+      </c>
+      <c r="L21" s="8">
+        <f>+L7/H7-1</f>
+        <v>-5.4322169059011216E-2</v>
+      </c>
+      <c r="M21" s="8">
+        <f>+M7/I7-1</f>
+        <v>1.9391623069452635E-2</v>
+      </c>
+      <c r="N21" s="8">
+        <f>+N7/J7-1</f>
+        <v>-3.3244680851063357E-4</v>
+      </c>
+      <c r="O21" s="8">
+        <f>+O7/K7-1</f>
+        <v>9.6195135686881761E-2</v>
+      </c>
+      <c r="P21" s="8">
+        <f>+P7/L7-1</f>
+        <v>0.14871656491381935</v>
+      </c>
+      <c r="Q21" s="8">
+        <f>+Q7/M7-1</f>
+        <v>5.8604794099569757E-2</v>
+      </c>
+      <c r="R21" s="8">
+        <f>+R7/N7-1</f>
+        <v>5.6655682196087964E-2</v>
+      </c>
+      <c r="S21" s="8">
+        <f>+S7/O7-1</f>
+        <v>1.1848189057282354E-2</v>
+      </c>
+      <c r="T21" s="8">
+        <f>+T7/P7-1</f>
+        <v>-3.670425182053072E-3</v>
+      </c>
+      <c r="U21" s="8">
+        <f>+U7/Q7-1</f>
+        <v>0</v>
+      </c>
+      <c r="V21" s="8">
+        <f>+V7/R7-1</f>
+        <v>0</v>
+      </c>
+      <c r="AN21" s="9">
+        <f>+AN7/AM7-1</f>
+        <v>-6.5706505586659025E-3</v>
+      </c>
+      <c r="AO21" s="9">
+        <f>+AO7/AN7-1</f>
+        <v>8.8320194057004198E-2</v>
+      </c>
+      <c r="AP21" s="9">
+        <f>+AP7/AO7-1</f>
+        <v>1.8128055394581732E-3</v>
+      </c>
+    </row>
+    <row r="22" spans="2:42" x14ac:dyDescent="0.2">
+      <c r="B22" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G22" s="8">
+        <f t="shared" ref="G22:T22" si="21">+G9/G7</f>
+        <v>0.46676619037463568</v>
+      </c>
+      <c r="H22" s="8">
+        <f t="shared" si="21"/>
+        <v>0.49291866028708137</v>
+      </c>
+      <c r="I22" s="8">
+        <f t="shared" si="21"/>
+        <v>0.49481532533441935</v>
+      </c>
+      <c r="J22" s="8">
+        <f t="shared" si="21"/>
+        <v>0.47748428433268858</v>
+      </c>
+      <c r="K22" s="8">
+        <f t="shared" si="21"/>
+        <v>0.45281757065925171</v>
+      </c>
+      <c r="L22" s="8">
+        <f t="shared" si="21"/>
+        <v>0.48827874658481463</v>
+      </c>
+      <c r="M22" s="8">
+        <f t="shared" si="21"/>
+        <v>0.4999078057775046</v>
+      </c>
+      <c r="N22" s="8">
+        <f t="shared" si="21"/>
+        <v>0.4877104936965263</v>
+      </c>
+      <c r="O22" s="8">
+        <f t="shared" si="21"/>
+        <v>0.51348574364243516</v>
+      </c>
+      <c r="P22" s="8">
+        <f t="shared" si="21"/>
+        <v>0.52528188865398173</v>
+      </c>
+      <c r="Q22" s="8">
+        <f t="shared" si="21"/>
+        <v>0.52698348187069988</v>
+      </c>
+      <c r="R22" s="8">
+        <f t="shared" si="21"/>
+        <v>0.5016451603673715</v>
+      </c>
+      <c r="S22" s="8">
+        <f t="shared" si="21"/>
+        <v>0.51477168152825814</v>
+      </c>
+      <c r="T22" s="8">
+        <f>+T9/T7</f>
+        <v>0.51672511862308801</v>
+      </c>
+      <c r="U22" s="8">
+        <f>+U9/U7</f>
+        <v>0.52</v>
+      </c>
+      <c r="V22" s="8">
+        <f>+V9/V7</f>
+        <v>0.52</v>
+      </c>
+      <c r="AN22" s="9"/>
+      <c r="AO22" s="9"/>
+      <c r="AP22" s="9"/>
+    </row>
+    <row r="24" spans="2:42" x14ac:dyDescent="0.2">
       <c r="B24" t="s">
         <v>48</v>
       </c>
@@ -1170,8 +2628,12 @@
         <f>+K25-K38</f>
         <v>171599</v>
       </c>
-    </row>
-    <row r="25" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="T24" s="1">
+        <f>+T25-T38</f>
+        <v>206143</v>
+      </c>
+    </row>
+    <row r="25" spans="2:42" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B25" s="1" t="s">
         <v>3</v>
       </c>
@@ -1190,8 +2652,12 @@
       <c r="L25" s="3"/>
       <c r="M25" s="3"/>
       <c r="N25" s="3"/>
-    </row>
-    <row r="26" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="T25" s="1">
+        <f>43534+11646+106821+46193+72497</f>
+        <v>280691</v>
+      </c>
+    </row>
+    <row r="26" spans="2:42" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B26" s="1" t="s">
         <v>38</v>
       </c>
@@ -1209,8 +2675,11 @@
       <c r="L26" s="3"/>
       <c r="M26" s="3"/>
       <c r="N26" s="3"/>
-    </row>
-    <row r="27" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="T26" s="1">
+        <v>11112</v>
+      </c>
+    </row>
+    <row r="27" spans="2:42" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B27" s="1" t="s">
         <v>39</v>
       </c>
@@ -1229,8 +2698,11 @@
       <c r="L27" s="3"/>
       <c r="M27" s="3"/>
       <c r="N27" s="3"/>
-    </row>
-    <row r="28" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="T27" s="1">
+        <v>1396</v>
+      </c>
+    </row>
+    <row r="28" spans="2:42" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B28" s="1" t="s">
         <v>43</v>
       </c>
@@ -1248,8 +2720,11 @@
       <c r="L28" s="3"/>
       <c r="M28" s="3"/>
       <c r="N28" s="3"/>
-    </row>
-    <row r="29" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="T28" s="1">
+        <v>12757</v>
+      </c>
+    </row>
+    <row r="29" spans="2:42" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B29" s="1" t="s">
         <v>41</v>
       </c>
@@ -1267,8 +2742,11 @@
       <c r="L29" s="3"/>
       <c r="M29" s="3"/>
       <c r="N29" s="3"/>
-    </row>
-    <row r="30" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="T29" s="1">
+        <v>29154</v>
+      </c>
+    </row>
+    <row r="30" spans="2:42" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B30" s="1" t="s">
         <v>35</v>
       </c>
@@ -1286,8 +2764,11 @@
       <c r="L30" s="3"/>
       <c r="M30" s="3"/>
       <c r="N30" s="3"/>
-    </row>
-    <row r="31" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="T30" s="1">
+        <v>6914</v>
+      </c>
+    </row>
+    <row r="31" spans="2:42" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B31" s="1" t="s">
         <v>36</v>
       </c>
@@ -1305,8 +2786,11 @@
       <c r="L31" s="3"/>
       <c r="M31" s="3"/>
       <c r="N31" s="3"/>
-    </row>
-    <row r="32" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="T31" s="1">
+        <v>14320</v>
+      </c>
+    </row>
+    <row r="32" spans="2:42" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B32" s="1" t="s">
         <v>37</v>
       </c>
@@ -1325,8 +2809,12 @@
       <c r="L32" s="3"/>
       <c r="M32" s="3"/>
       <c r="N32" s="3"/>
-    </row>
-    <row r="33" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="T32" s="1">
+        <f>812+22586</f>
+        <v>23398</v>
+      </c>
+    </row>
+    <row r="33" spans="2:41" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B33" s="1" t="s">
         <v>32</v>
       </c>
@@ -1344,8 +2832,11 @@
       <c r="L33" s="3"/>
       <c r="M33" s="3"/>
       <c r="N33" s="3"/>
-    </row>
-    <row r="34" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="T33" s="1">
+        <v>2342</v>
+      </c>
+    </row>
+    <row r="34" spans="2:41" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B34" s="1" t="s">
         <v>42</v>
       </c>
@@ -1363,8 +2854,11 @@
       <c r="L34" s="3"/>
       <c r="M34" s="3"/>
       <c r="N34" s="3"/>
-    </row>
-    <row r="35" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="T34" s="1">
+        <v>10919</v>
+      </c>
+    </row>
+    <row r="35" spans="2:41" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B35" s="1" t="s">
         <v>40</v>
       </c>
@@ -1382,8 +2876,12 @@
       <c r="L35" s="3"/>
       <c r="M35" s="3"/>
       <c r="N35" s="3"/>
-    </row>
-    <row r="36" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="T35" s="1">
+        <f>22312+212</f>
+        <v>22524</v>
+      </c>
+    </row>
+    <row r="36" spans="2:41" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B36" s="1" t="s">
         <v>44</v>
       </c>
@@ -1399,11 +2897,44 @@
         <f>SUM(K25:K35)</f>
         <v>375633</v>
       </c>
-      <c r="L36" s="3"/>
-      <c r="M36" s="3"/>
-      <c r="N36" s="3"/>
-    </row>
-    <row r="38" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="L36" s="3">
+        <f t="shared" ref="L36:T46" si="22">SUM(L25:L35)</f>
+        <v>0</v>
+      </c>
+      <c r="M36" s="3">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="N36" s="3">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="O36" s="3">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="P36" s="3">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="Q36" s="3">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="R36" s="3">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="S36" s="3">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="T36" s="3">
+        <f t="shared" si="22"/>
+        <v>415527</v>
+      </c>
+    </row>
+    <row r="38" spans="2:41" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B38" s="1" t="s">
         <v>4</v>
       </c>
@@ -1422,8 +2953,12 @@
       <c r="L38" s="3"/>
       <c r="M38" s="3"/>
       <c r="N38" s="3"/>
-    </row>
-    <row r="39" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="T38" s="3">
+        <f>12514+29+2892+7986+14859+27860+8408</f>
+        <v>74548</v>
+      </c>
+    </row>
+    <row r="39" spans="2:41" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B39" s="1" t="s">
         <v>46</v>
       </c>
@@ -1441,8 +2976,11 @@
       <c r="L39" s="3"/>
       <c r="M39" s="3"/>
       <c r="N39" s="3"/>
-    </row>
-    <row r="40" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="T39" s="3">
+        <v>37988</v>
+      </c>
+    </row>
+    <row r="40" spans="2:41" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B40" s="1" t="s">
         <v>45</v>
       </c>
@@ -1461,8 +2999,12 @@
       <c r="L40" s="3"/>
       <c r="M40" s="3"/>
       <c r="N40" s="3"/>
-    </row>
-    <row r="41" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="T40" s="3">
+        <f>14038+291+287+520</f>
+        <v>15136</v>
+      </c>
+    </row>
+    <row r="41" spans="2:41" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B41" s="1" t="s">
         <v>47</v>
       </c>
@@ -1480,8 +3022,12 @@
       <c r="L41" s="3"/>
       <c r="M41" s="3"/>
       <c r="N41" s="3"/>
-    </row>
-    <row r="42" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="T41" s="3">
+        <f>1831+67</f>
+        <v>1898</v>
+      </c>
+    </row>
+    <row r="42" spans="2:41" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B42" s="1" t="s">
         <v>42</v>
       </c>
@@ -1500,8 +3046,12 @@
       <c r="L42" s="3"/>
       <c r="M42" s="3"/>
       <c r="N42" s="3"/>
-    </row>
-    <row r="43" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="T42" s="3">
+        <f>3196+5056</f>
+        <v>8252</v>
+      </c>
+    </row>
+    <row r="43" spans="2:41" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B43" s="1" t="s">
         <v>32</v>
       </c>
@@ -1519,8 +3069,11 @@
       <c r="L43" s="3"/>
       <c r="M43" s="3"/>
       <c r="N43" s="3"/>
-    </row>
-    <row r="44" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="T43" s="3">
+        <v>2940</v>
+      </c>
+    </row>
+    <row r="44" spans="2:41" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B44" s="1" t="s">
         <v>51</v>
       </c>
@@ -1538,8 +3091,11 @@
       <c r="L44" s="3"/>
       <c r="M44" s="3"/>
       <c r="N44" s="3"/>
-    </row>
-    <row r="45" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="T44" s="3">
+        <v>1827</v>
+      </c>
+    </row>
+    <row r="45" spans="2:41" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B45" s="1" t="s">
         <v>50</v>
       </c>
@@ -1558,8 +3114,12 @@
       <c r="L45" s="3"/>
       <c r="M45" s="3"/>
       <c r="N45" s="3"/>
-    </row>
-    <row r="46" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="T45" s="3">
+        <f>262831+10107</f>
+        <v>272938</v>
+      </c>
+    </row>
+    <row r="46" spans="2:41" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B46" s="1" t="s">
         <v>49</v>
       </c>
@@ -1578,6 +3138,81 @@
       <c r="L46" s="3"/>
       <c r="M46" s="3"/>
       <c r="N46" s="3"/>
+      <c r="T46" s="3">
+        <f>SUM(T38:T45)</f>
+        <v>415527</v>
+      </c>
+    </row>
+    <row r="48" spans="2:41" x14ac:dyDescent="0.2">
+      <c r="B48" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="P48" s="1">
+        <v>9746</v>
+      </c>
+      <c r="Q48" s="1"/>
+      <c r="R48" s="1"/>
+      <c r="S48" s="1">
+        <v>5284</v>
+      </c>
+      <c r="T48" s="1">
+        <v>7970</v>
+      </c>
+      <c r="AN48" s="1">
+        <v>26241</v>
+      </c>
+      <c r="AO48" s="1">
+        <v>33263</v>
+      </c>
+    </row>
+    <row r="49" spans="2:41" x14ac:dyDescent="0.2">
+      <c r="B49" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="P49" s="1">
+        <v>2693</v>
+      </c>
+      <c r="Q49" s="1"/>
+      <c r="R49" s="1"/>
+      <c r="S49" s="1">
+        <v>2016</v>
+      </c>
+      <c r="T49" s="1">
+        <v>2090</v>
+      </c>
+      <c r="AN49" s="1">
+        <v>8112</v>
+      </c>
+      <c r="AO49" s="1">
+        <v>11154</v>
+      </c>
+    </row>
+    <row r="50" spans="2:41" x14ac:dyDescent="0.2">
+      <c r="B50" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="P50" s="1">
+        <f>+P48-P49</f>
+        <v>7053</v>
+      </c>
+      <c r="Q50" s="1"/>
+      <c r="R50" s="1"/>
+      <c r="S50" s="1">
+        <f>+S48-S49</f>
+        <v>3268</v>
+      </c>
+      <c r="T50" s="1">
+        <f>+T48-T49</f>
+        <v>5880</v>
+      </c>
+      <c r="AN50" s="4">
+        <f>+AN48-AN49</f>
+        <v>18129</v>
+      </c>
+      <c r="AO50" s="4">
+        <f>+AO48-AO49</f>
+        <v>22109</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>